<commit_message>
Wrote Script to Scrape Home Run Data
</commit_message>
<xml_diff>
--- a/FINAL_HITTER_DKPTS_PREDICTIONS.xlsx
+++ b/FINAL_HITTER_DKPTS_PREDICTIONS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="202">
   <si>
     <t>Batter</t>
   </si>
@@ -957,7 +957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1003,10 +1003,10 @@
         <v>2100</v>
       </c>
       <c r="F2" s="1">
-        <v>7.95</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2">
-        <v>3.7857</v>
+        <v>4.2857</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1026,10 +1026,10 @@
         <v>3900</v>
       </c>
       <c r="F3" s="1">
-        <v>8.98</v>
+        <v>9.17</v>
       </c>
       <c r="G3" s="2">
-        <v>2.3026</v>
+        <v>2.3513</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1049,10 +1049,10 @@
         <v>3500</v>
       </c>
       <c r="F4" s="1">
-        <v>8.57</v>
+        <v>8.56</v>
       </c>
       <c r="G4" s="2">
-        <v>2.4486</v>
+        <v>2.4457</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1072,10 +1072,10 @@
         <v>3900</v>
       </c>
       <c r="F5" s="1">
-        <v>8.42</v>
+        <v>7.9</v>
       </c>
       <c r="G5" s="2">
-        <v>2.159</v>
+        <v>2.0256</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1095,10 +1095,10 @@
         <v>3100</v>
       </c>
       <c r="F6" s="1">
-        <v>9.19</v>
+        <v>7.54</v>
       </c>
       <c r="G6" s="2">
-        <v>2.9645</v>
+        <v>2.4323</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1118,10 +1118,10 @@
         <v>2100</v>
       </c>
       <c r="F7" s="1">
-        <v>7.9</v>
+        <v>6.8</v>
       </c>
       <c r="G7" s="2">
-        <v>3.7619</v>
+        <v>3.2381</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1141,10 +1141,10 @@
         <v>4100</v>
       </c>
       <c r="F8" s="1">
-        <v>6.78</v>
+        <v>6.16</v>
       </c>
       <c r="G8" s="2">
-        <v>1.6537</v>
+        <v>1.5024</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1164,10 +1164,10 @@
         <v>2800</v>
       </c>
       <c r="F9" s="1">
-        <v>7.91</v>
+        <v>6.95</v>
       </c>
       <c r="G9" s="2">
-        <v>2.825</v>
+        <v>2.4821</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1187,10 +1187,10 @@
         <v>3500</v>
       </c>
       <c r="F10" s="1">
-        <v>6.34</v>
+        <v>6.03</v>
       </c>
       <c r="G10" s="2">
-        <v>1.8114</v>
+        <v>1.7229</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1210,10 +1210,10 @@
         <v>3000</v>
       </c>
       <c r="F11" s="1">
-        <v>7.89</v>
+        <v>8.130000000000001</v>
       </c>
       <c r="G11" s="2">
-        <v>2.63</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1233,10 +1233,10 @@
         <v>3900</v>
       </c>
       <c r="F12" s="1">
-        <v>7.92</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="G12" s="2">
-        <v>2.0308</v>
+        <v>2.1282</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1256,10 +1256,10 @@
         <v>4300</v>
       </c>
       <c r="F13" s="1">
-        <v>8.539999999999999</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="G13" s="2">
-        <v>1.986</v>
+        <v>2.0233</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1279,10 +1279,10 @@
         <v>5400</v>
       </c>
       <c r="F14" s="1">
-        <v>8.359999999999999</v>
+        <v>8.25</v>
       </c>
       <c r="G14" s="2">
-        <v>1.5481</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1302,10 +1302,10 @@
         <v>5400</v>
       </c>
       <c r="F15" s="1">
-        <v>8.609999999999999</v>
+        <v>7.72</v>
       </c>
       <c r="G15" s="2">
-        <v>1.5944</v>
+        <v>1.4296</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1325,10 +1325,10 @@
         <v>3200</v>
       </c>
       <c r="F16" s="1">
-        <v>7.08</v>
+        <v>6.87</v>
       </c>
       <c r="G16" s="2">
-        <v>2.2125</v>
+        <v>2.1469</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1348,10 +1348,10 @@
         <v>3300</v>
       </c>
       <c r="F17" s="1">
-        <v>6.16</v>
+        <v>6.41</v>
       </c>
       <c r="G17" s="2">
-        <v>1.8667</v>
+        <v>1.9424</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1371,10 +1371,10 @@
         <v>4700</v>
       </c>
       <c r="F18" s="1">
-        <v>5.89</v>
+        <v>6.41</v>
       </c>
       <c r="G18" s="2">
-        <v>1.2532</v>
+        <v>1.3638</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1394,10 +1394,10 @@
         <v>4000</v>
       </c>
       <c r="F19" s="1">
-        <v>7.05</v>
+        <v>6.04</v>
       </c>
       <c r="G19" s="2">
-        <v>1.7625</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1417,10 +1417,10 @@
         <v>3800</v>
       </c>
       <c r="F20" s="1">
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
       <c r="G20" s="2">
-        <v>1.7105</v>
+        <v>1.7763</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1440,10 +1440,10 @@
         <v>4500</v>
       </c>
       <c r="F21" s="1">
-        <v>6.78</v>
+        <v>6.8</v>
       </c>
       <c r="G21" s="2">
-        <v>1.5067</v>
+        <v>1.5111</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1463,10 +1463,10 @@
         <v>3300</v>
       </c>
       <c r="F22" s="1">
-        <v>7.24</v>
+        <v>6.71</v>
       </c>
       <c r="G22" s="2">
-        <v>2.1939</v>
+        <v>2.0333</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1486,10 +1486,10 @@
         <v>3700</v>
       </c>
       <c r="F23" s="1">
-        <v>8.68</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="G23" s="2">
-        <v>2.3459</v>
+        <v>2.1757</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1509,10 +1509,10 @@
         <v>3700</v>
       </c>
       <c r="F24" s="1">
-        <v>7.11</v>
+        <v>6.5</v>
       </c>
       <c r="G24" s="2">
-        <v>1.9216</v>
+        <v>1.7568</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1532,10 +1532,10 @@
         <v>4200</v>
       </c>
       <c r="F25" s="1">
-        <v>6.12</v>
+        <v>6.08</v>
       </c>
       <c r="G25" s="2">
-        <v>1.4571</v>
+        <v>1.4476</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1555,10 +1555,10 @@
         <v>2400</v>
       </c>
       <c r="F26" s="1">
-        <v>7.71</v>
+        <v>6.49</v>
       </c>
       <c r="G26" s="2">
-        <v>3.2125</v>
+        <v>2.7042</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1578,10 +1578,10 @@
         <v>2400</v>
       </c>
       <c r="F27" s="1">
-        <v>5.05</v>
+        <v>5.54</v>
       </c>
       <c r="G27" s="2">
-        <v>2.1042</v>
+        <v>2.3083</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1617,10 +1617,10 @@
         <v>4100</v>
       </c>
       <c r="F29" s="1">
-        <v>7.5</v>
+        <v>7.17</v>
       </c>
       <c r="G29" s="2">
-        <v>1.8293</v>
+        <v>1.7488</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1640,10 +1640,10 @@
         <v>3200</v>
       </c>
       <c r="F30" s="1">
-        <v>7.28</v>
+        <v>7.45</v>
       </c>
       <c r="G30" s="2">
-        <v>2.275</v>
+        <v>2.3281</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1663,10 +1663,10 @@
         <v>5600</v>
       </c>
       <c r="F31" s="1">
-        <v>7.89</v>
+        <v>7.84</v>
       </c>
       <c r="G31" s="2">
-        <v>1.4089</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1686,10 +1686,10 @@
         <v>4700</v>
       </c>
       <c r="F32" s="1">
-        <v>7.59</v>
+        <v>7.53</v>
       </c>
       <c r="G32" s="2">
-        <v>1.6149</v>
+        <v>1.6021</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1709,10 +1709,10 @@
         <v>4600</v>
       </c>
       <c r="F33" s="1">
-        <v>6.76</v>
+        <v>6.57</v>
       </c>
       <c r="G33" s="2">
-        <v>1.4696</v>
+        <v>1.4283</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1732,10 +1732,10 @@
         <v>4100</v>
       </c>
       <c r="F34" s="1">
-        <v>6.26</v>
+        <v>6.18</v>
       </c>
       <c r="G34" s="2">
-        <v>1.5268</v>
+        <v>1.5073</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1755,10 +1755,10 @@
         <v>3000</v>
       </c>
       <c r="F35" s="1">
-        <v>5.85</v>
+        <v>5.51</v>
       </c>
       <c r="G35" s="2">
-        <v>1.95</v>
+        <v>1.8367</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1778,10 +1778,10 @@
         <v>3000</v>
       </c>
       <c r="F36" s="1">
-        <v>5.06</v>
+        <v>5.17</v>
       </c>
       <c r="G36" s="2">
-        <v>1.6867</v>
+        <v>1.7233</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1817,10 +1817,10 @@
         <v>3400</v>
       </c>
       <c r="F38" s="1">
-        <v>6.28</v>
+        <v>6.69</v>
       </c>
       <c r="G38" s="2">
-        <v>1.8471</v>
+        <v>1.9676</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1863,10 +1863,10 @@
         <v>3200</v>
       </c>
       <c r="F40" s="1">
-        <v>7.41</v>
+        <v>6.96</v>
       </c>
       <c r="G40" s="2">
-        <v>2.3156</v>
+        <v>2.175</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1886,10 +1886,10 @@
         <v>3400</v>
       </c>
       <c r="F41" s="1">
-        <v>7.36</v>
+        <v>6.92</v>
       </c>
       <c r="G41" s="2">
-        <v>2.1647</v>
+        <v>2.0353</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1909,10 +1909,10 @@
         <v>2900</v>
       </c>
       <c r="F42" s="1">
-        <v>6.64</v>
+        <v>6.46</v>
       </c>
       <c r="G42" s="2">
-        <v>2.2897</v>
+        <v>2.2276</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1932,10 +1932,10 @@
         <v>3200</v>
       </c>
       <c r="F43" s="1">
-        <v>5.83</v>
+        <v>6.49</v>
       </c>
       <c r="G43" s="2">
-        <v>1.8219</v>
+        <v>2.0281</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1955,10 +1955,10 @@
         <v>3000</v>
       </c>
       <c r="F44" s="1">
-        <v>5.47</v>
+        <v>6.26</v>
       </c>
       <c r="G44" s="2">
-        <v>1.8233</v>
+        <v>2.0867</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1978,10 +1978,10 @@
         <v>2800</v>
       </c>
       <c r="F45" s="1">
-        <v>5.72</v>
+        <v>5.06</v>
       </c>
       <c r="G45" s="2">
-        <v>2.0429</v>
+        <v>1.8071</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2017,10 +2017,10 @@
         <v>4400</v>
       </c>
       <c r="F47" s="1">
-        <v>8.539999999999999</v>
+        <v>8.26</v>
       </c>
       <c r="G47" s="2">
-        <v>1.9409</v>
+        <v>1.8773</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2040,10 +2040,10 @@
         <v>5000</v>
       </c>
       <c r="F48" s="1">
-        <v>8.08</v>
+        <v>7.48</v>
       </c>
       <c r="G48" s="2">
-        <v>1.616</v>
+        <v>1.496</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2063,10 +2063,10 @@
         <v>4800</v>
       </c>
       <c r="F49" s="1">
-        <v>7.2</v>
+        <v>7.27</v>
       </c>
       <c r="G49" s="2">
-        <v>1.5</v>
+        <v>1.5146</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2086,10 +2086,10 @@
         <v>5000</v>
       </c>
       <c r="F50" s="1">
-        <v>7.26</v>
+        <v>7.14</v>
       </c>
       <c r="G50" s="2">
-        <v>1.452</v>
+        <v>1.428</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2109,10 +2109,10 @@
         <v>3400</v>
       </c>
       <c r="F51" s="1">
-        <v>7.04</v>
+        <v>6.96</v>
       </c>
       <c r="G51" s="2">
-        <v>2.0706</v>
+        <v>2.0471</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2132,10 +2132,10 @@
         <v>5100</v>
       </c>
       <c r="F52" s="1">
-        <v>7.25</v>
+        <v>6.63</v>
       </c>
       <c r="G52" s="2">
-        <v>1.4216</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2155,10 +2155,10 @@
         <v>3800</v>
       </c>
       <c r="F53" s="1">
-        <v>5.73</v>
+        <v>5.75</v>
       </c>
       <c r="G53" s="2">
-        <v>1.5079</v>
+        <v>1.5132</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2178,10 +2178,10 @@
         <v>3200</v>
       </c>
       <c r="F54" s="1">
-        <v>4.88</v>
+        <v>5.34</v>
       </c>
       <c r="G54" s="2">
-        <v>1.525</v>
+        <v>1.6687</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2217,10 +2217,10 @@
         <v>6000</v>
       </c>
       <c r="F56" s="1">
-        <v>8.18</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="G56" s="2">
-        <v>1.3633</v>
+        <v>1.3817</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2240,10 +2240,10 @@
         <v>5000</v>
       </c>
       <c r="F57" s="1">
-        <v>8.23</v>
+        <v>7.76</v>
       </c>
       <c r="G57" s="2">
-        <v>1.646</v>
+        <v>1.552</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2263,10 +2263,10 @@
         <v>5400</v>
       </c>
       <c r="F58" s="1">
-        <v>8.01</v>
+        <v>8.19</v>
       </c>
       <c r="G58" s="2">
-        <v>1.4833</v>
+        <v>1.5167</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2286,10 +2286,10 @@
         <v>5400</v>
       </c>
       <c r="F59" s="1">
-        <v>7.84</v>
+        <v>7.82</v>
       </c>
       <c r="G59" s="2">
-        <v>1.4519</v>
+        <v>1.4481</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2309,10 +2309,10 @@
         <v>4800</v>
       </c>
       <c r="F60" s="1">
-        <v>7.55</v>
+        <v>6.58</v>
       </c>
       <c r="G60" s="2">
-        <v>1.5729</v>
+        <v>1.3708</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2332,10 +2332,10 @@
         <v>5000</v>
       </c>
       <c r="F61" s="1">
-        <v>6.98</v>
+        <v>5.98</v>
       </c>
       <c r="G61" s="2">
-        <v>1.396</v>
+        <v>1.196</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2355,10 +2355,10 @@
         <v>4300</v>
       </c>
       <c r="F62" s="1">
-        <v>6.62</v>
+        <v>6.78</v>
       </c>
       <c r="G62" s="2">
-        <v>1.5395</v>
+        <v>1.5767</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2378,10 +2378,10 @@
         <v>3500</v>
       </c>
       <c r="F63" s="1">
-        <v>7.26</v>
+        <v>6.09</v>
       </c>
       <c r="G63" s="2">
-        <v>2.0743</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2417,10 +2417,10 @@
         <v>3900</v>
       </c>
       <c r="F65" s="1">
-        <v>6.68</v>
+        <v>7.29</v>
       </c>
       <c r="G65" s="2">
-        <v>1.7128</v>
+        <v>1.8692</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2440,10 +2440,10 @@
         <v>5000</v>
       </c>
       <c r="F66" s="1">
-        <v>6.88</v>
+        <v>7.39</v>
       </c>
       <c r="G66" s="2">
-        <v>1.376</v>
+        <v>1.478</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2463,10 +2463,10 @@
         <v>5500</v>
       </c>
       <c r="F67" s="1">
-        <v>7.69</v>
+        <v>6.92</v>
       </c>
       <c r="G67" s="2">
-        <v>1.3982</v>
+        <v>1.2582</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2486,10 +2486,10 @@
         <v>5500</v>
       </c>
       <c r="F68" s="1">
-        <v>7.76</v>
+        <v>6.96</v>
       </c>
       <c r="G68" s="2">
-        <v>1.4109</v>
+        <v>1.2655</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2509,10 +2509,10 @@
         <v>3100</v>
       </c>
       <c r="F69" s="1">
-        <v>7.48</v>
+        <v>6.74</v>
       </c>
       <c r="G69" s="2">
-        <v>2.4129</v>
+        <v>2.1742</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2532,10 +2532,10 @@
         <v>4800</v>
       </c>
       <c r="F70" s="1">
-        <v>6.99</v>
+        <v>6.45</v>
       </c>
       <c r="G70" s="2">
-        <v>1.4563</v>
+        <v>1.3438</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2555,10 +2555,10 @@
         <v>4500</v>
       </c>
       <c r="F71" s="1">
-        <v>5.88</v>
+        <v>5.59</v>
       </c>
       <c r="G71" s="2">
-        <v>1.3067</v>
+        <v>1.2422</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2578,10 +2578,10 @@
         <v>2900</v>
       </c>
       <c r="F72" s="1">
-        <v>4.58</v>
+        <v>5.23</v>
       </c>
       <c r="G72" s="2">
-        <v>1.5793</v>
+        <v>1.8034</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2617,10 +2617,10 @@
         <v>3300</v>
       </c>
       <c r="F74" s="1">
-        <v>8.74</v>
+        <v>7.63</v>
       </c>
       <c r="G74" s="2">
-        <v>2.6485</v>
+        <v>2.3121</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2640,10 +2640,10 @@
         <v>5300</v>
       </c>
       <c r="F75" s="1">
-        <v>9.18</v>
+        <v>7.96</v>
       </c>
       <c r="G75" s="2">
-        <v>1.7321</v>
+        <v>1.5019</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2663,10 +2663,10 @@
         <v>3600</v>
       </c>
       <c r="F76" s="1">
-        <v>7.72</v>
+        <v>7.37</v>
       </c>
       <c r="G76" s="2">
-        <v>2.1444</v>
+        <v>2.0472</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2686,10 +2686,10 @@
         <v>4600</v>
       </c>
       <c r="F77" s="1">
-        <v>7.99</v>
+        <v>7.32</v>
       </c>
       <c r="G77" s="2">
-        <v>1.737</v>
+        <v>1.5913</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2709,10 +2709,10 @@
         <v>4900</v>
       </c>
       <c r="F78" s="1">
-        <v>7.07</v>
+        <v>6.79</v>
       </c>
       <c r="G78" s="2">
-        <v>1.4429</v>
+        <v>1.3857</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2732,10 +2732,10 @@
         <v>4100</v>
       </c>
       <c r="F79" s="1">
-        <v>6.69</v>
+        <v>6.06</v>
       </c>
       <c r="G79" s="2">
-        <v>1.6317</v>
+        <v>1.478</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2755,10 +2755,10 @@
         <v>2900</v>
       </c>
       <c r="F80" s="1">
-        <v>6.7</v>
+        <v>6.13</v>
       </c>
       <c r="G80" s="2">
-        <v>2.3103</v>
+        <v>2.1138</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2778,10 +2778,10 @@
         <v>4100</v>
       </c>
       <c r="F81" s="1">
-        <v>4.87</v>
+        <v>5.5</v>
       </c>
       <c r="G81" s="2">
-        <v>1.1878</v>
+        <v>1.3415</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2817,10 +2817,10 @@
         <v>2700</v>
       </c>
       <c r="F83" s="1">
-        <v>7.3</v>
+        <v>6.76</v>
       </c>
       <c r="G83" s="2">
-        <v>2.7037</v>
+        <v>2.5037</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2840,10 +2840,10 @@
         <v>4900</v>
       </c>
       <c r="F84" s="1">
-        <v>6.92</v>
+        <v>7.21</v>
       </c>
       <c r="G84" s="2">
-        <v>1.4122</v>
+        <v>1.4714</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2863,10 +2863,10 @@
         <v>3500</v>
       </c>
       <c r="F85" s="1">
-        <v>7</v>
+        <v>7.09</v>
       </c>
       <c r="G85" s="2">
-        <v>2</v>
+        <v>2.0257</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2886,10 +2886,10 @@
         <v>3400</v>
       </c>
       <c r="F86" s="1">
-        <v>8.109999999999999</v>
+        <v>7.2</v>
       </c>
       <c r="G86" s="2">
-        <v>2.3853</v>
+        <v>2.1176</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2909,10 +2909,10 @@
         <v>3400</v>
       </c>
       <c r="F87" s="1">
-        <v>6.89</v>
+        <v>6.96</v>
       </c>
       <c r="G87" s="2">
-        <v>2.0265</v>
+        <v>2.0471</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2932,10 +2932,10 @@
         <v>2500</v>
       </c>
       <c r="F88" s="1">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="G88" s="2">
-        <v>2.32</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2955,10 +2955,10 @@
         <v>2400</v>
       </c>
       <c r="F89" s="1">
-        <v>6.54</v>
+        <v>5.81</v>
       </c>
       <c r="G89" s="2">
-        <v>2.725</v>
+        <v>2.4208</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2978,10 +2978,10 @@
         <v>3400</v>
       </c>
       <c r="F90" s="1">
-        <v>4.64</v>
+        <v>5.15</v>
       </c>
       <c r="G90" s="2">
-        <v>1.3647</v>
+        <v>1.5147</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -3017,10 +3017,10 @@
         <v>4200</v>
       </c>
       <c r="F92" s="1">
-        <v>8.02</v>
+        <v>7.71</v>
       </c>
       <c r="G92" s="2">
-        <v>1.9095</v>
+        <v>1.8357</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3040,10 +3040,10 @@
         <v>5100</v>
       </c>
       <c r="F93" s="1">
-        <v>8.210000000000001</v>
+        <v>7.62</v>
       </c>
       <c r="G93" s="2">
-        <v>1.6098</v>
+        <v>1.4941</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3063,10 +3063,10 @@
         <v>5300</v>
       </c>
       <c r="F94" s="1">
-        <v>6.97</v>
+        <v>7.68</v>
       </c>
       <c r="G94" s="2">
-        <v>1.3151</v>
+        <v>1.4491</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3086,10 +3086,10 @@
         <v>4400</v>
       </c>
       <c r="F95" s="1">
-        <v>6.38</v>
+        <v>7.24</v>
       </c>
       <c r="G95" s="2">
-        <v>1.45</v>
+        <v>1.6455</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3109,10 +3109,10 @@
         <v>3400</v>
       </c>
       <c r="F96" s="1">
-        <v>6.18</v>
+        <v>6.34</v>
       </c>
       <c r="G96" s="2">
-        <v>1.8176</v>
+        <v>1.8647</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -3132,10 +3132,10 @@
         <v>2900</v>
       </c>
       <c r="F97" s="1">
-        <v>6.09</v>
+        <v>5.86</v>
       </c>
       <c r="G97" s="2">
-        <v>2.1</v>
+        <v>2.0207</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -3155,10 +3155,10 @@
         <v>3300</v>
       </c>
       <c r="F98" s="1">
-        <v>5.92</v>
+        <v>6.43</v>
       </c>
       <c r="G98" s="2">
-        <v>1.7939</v>
+        <v>1.9485</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -3178,10 +3178,10 @@
         <v>2100</v>
       </c>
       <c r="F99" s="1">
-        <v>5.36</v>
+        <v>5.32</v>
       </c>
       <c r="G99" s="2">
-        <v>2.5524</v>
+        <v>2.5333</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -3217,10 +3217,10 @@
         <v>4000</v>
       </c>
       <c r="F101" s="1">
-        <v>8.58</v>
+        <v>7.34</v>
       </c>
       <c r="G101" s="2">
-        <v>2.145</v>
+        <v>1.835</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3240,10 +3240,10 @@
         <v>5100</v>
       </c>
       <c r="F102" s="1">
-        <v>8.24</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="G102" s="2">
-        <v>1.6157</v>
+        <v>1.6275</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3263,10 +3263,10 @@
         <v>4700</v>
       </c>
       <c r="F103" s="1">
-        <v>6.8</v>
+        <v>7.15</v>
       </c>
       <c r="G103" s="2">
-        <v>1.4468</v>
+        <v>1.5213</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3286,10 +3286,10 @@
         <v>4000</v>
       </c>
       <c r="F104" s="1">
-        <v>6.25</v>
+        <v>7.83</v>
       </c>
       <c r="G104" s="2">
-        <v>1.5625</v>
+        <v>1.9575</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3309,10 +3309,10 @@
         <v>4000</v>
       </c>
       <c r="F105" s="1">
-        <v>7.33</v>
+        <v>6.69</v>
       </c>
       <c r="G105" s="2">
-        <v>1.8325</v>
+        <v>1.6725</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3332,10 +3332,10 @@
         <v>2700</v>
       </c>
       <c r="F106" s="1">
-        <v>7.14</v>
+        <v>6.25</v>
       </c>
       <c r="G106" s="2">
-        <v>2.6444</v>
+        <v>2.3148</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3355,10 +3355,10 @@
         <v>2400</v>
       </c>
       <c r="F107" s="1">
-        <v>6.66</v>
+        <v>5.61</v>
       </c>
       <c r="G107" s="2">
-        <v>2.775</v>
+        <v>2.3375</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3378,10 +3378,10 @@
         <v>3200</v>
       </c>
       <c r="F108" s="1">
-        <v>5.66</v>
+        <v>4.9</v>
       </c>
       <c r="G108" s="2">
-        <v>1.7688</v>
+        <v>1.5312</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3417,10 +3417,10 @@
         <v>5900</v>
       </c>
       <c r="F110" s="1">
-        <v>9.039999999999999</v>
+        <v>10.54</v>
       </c>
       <c r="G110" s="2">
-        <v>1.5322</v>
+        <v>1.7864</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3440,10 +3440,10 @@
         <v>5600</v>
       </c>
       <c r="F111" s="1">
-        <v>9.43</v>
+        <v>11.38</v>
       </c>
       <c r="G111" s="2">
-        <v>1.6839</v>
+        <v>2.0321</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3463,10 +3463,10 @@
         <v>4700</v>
       </c>
       <c r="F112" s="1">
-        <v>9.029999999999999</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="G112" s="2">
-        <v>1.9213</v>
+        <v>2.0277</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3486,10 +3486,10 @@
         <v>5800</v>
       </c>
       <c r="F113" s="1">
-        <v>8.42</v>
+        <v>8.1</v>
       </c>
       <c r="G113" s="2">
-        <v>1.4517</v>
+        <v>1.3966</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3509,10 +3509,10 @@
         <v>5200</v>
       </c>
       <c r="F114" s="1">
-        <v>7.4</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="G114" s="2">
-        <v>1.4231</v>
+        <v>1.6404</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3532,10 +3532,10 @@
         <v>4600</v>
       </c>
       <c r="F115" s="1">
-        <v>7.08</v>
+        <v>7.44</v>
       </c>
       <c r="G115" s="2">
-        <v>1.5391</v>
+        <v>1.6174</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3571,10 +3571,10 @@
         <v>3800</v>
       </c>
       <c r="F117" s="1">
-        <v>5.73</v>
+        <v>6.96</v>
       </c>
       <c r="G117" s="2">
-        <v>1.5079</v>
+        <v>1.8316</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3594,10 +3594,10 @@
         <v>4600</v>
       </c>
       <c r="F118" s="1">
-        <v>8.33</v>
+        <v>7.27</v>
       </c>
       <c r="G118" s="2">
-        <v>1.8109</v>
+        <v>1.5804</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3633,10 +3633,10 @@
         <v>3400</v>
       </c>
       <c r="F120" s="1">
-        <v>9.31</v>
+        <v>10.12</v>
       </c>
       <c r="G120" s="2">
-        <v>2.7382</v>
+        <v>2.9765</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3656,10 +3656,10 @@
         <v>3600</v>
       </c>
       <c r="F121" s="1">
-        <v>10.52</v>
+        <v>11.06</v>
       </c>
       <c r="G121" s="2">
-        <v>2.9222</v>
+        <v>3.0722</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3679,10 +3679,10 @@
         <v>5500</v>
       </c>
       <c r="F122" s="1">
-        <v>10.16</v>
+        <v>10.5</v>
       </c>
       <c r="G122" s="2">
-        <v>1.8473</v>
+        <v>1.9091</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3702,10 +3702,10 @@
         <v>5000</v>
       </c>
       <c r="F123" s="1">
-        <v>10.07</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="G123" s="2">
-        <v>2.014</v>
+        <v>1.928</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3725,10 +3725,10 @@
         <v>3800</v>
       </c>
       <c r="F124" s="1">
-        <v>9.09</v>
+        <v>9.460000000000001</v>
       </c>
       <c r="G124" s="2">
-        <v>2.3921</v>
+        <v>2.4895</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3748,10 +3748,10 @@
         <v>2900</v>
       </c>
       <c r="F125" s="1">
-        <v>7.64</v>
+        <v>6.3</v>
       </c>
       <c r="G125" s="2">
-        <v>2.6345</v>
+        <v>2.1724</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3771,10 +3771,10 @@
         <v>3400</v>
       </c>
       <c r="F126" s="1">
-        <v>8.23</v>
+        <v>5.67</v>
       </c>
       <c r="G126" s="2">
-        <v>2.4206</v>
+        <v>1.6676</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3794,10 +3794,10 @@
         <v>2700</v>
       </c>
       <c r="F127" s="1">
-        <v>7.65</v>
+        <v>6.56</v>
       </c>
       <c r="G127" s="2">
-        <v>2.8333</v>
+        <v>2.4296</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3833,10 +3833,10 @@
         <v>2800</v>
       </c>
       <c r="F129" s="1">
-        <v>7.58</v>
+        <v>7.75</v>
       </c>
       <c r="G129" s="2">
-        <v>2.7071</v>
+        <v>2.7679</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3856,10 +3856,10 @@
         <v>2700</v>
       </c>
       <c r="F130" s="1">
-        <v>7.41</v>
+        <v>7.34</v>
       </c>
       <c r="G130" s="2">
-        <v>2.7444</v>
+        <v>2.7185</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3879,10 +3879,10 @@
         <v>2800</v>
       </c>
       <c r="F131" s="1">
-        <v>6.81</v>
+        <v>7.14</v>
       </c>
       <c r="G131" s="2">
-        <v>2.4321</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3902,10 +3902,10 @@
         <v>3800</v>
       </c>
       <c r="F132" s="1">
-        <v>7.33</v>
+        <v>6.76</v>
       </c>
       <c r="G132" s="2">
-        <v>1.9289</v>
+        <v>1.7789</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3925,10 +3925,10 @@
         <v>2600</v>
       </c>
       <c r="F133" s="1">
-        <v>6.17</v>
+        <v>6.35</v>
       </c>
       <c r="G133" s="2">
-        <v>2.3731</v>
+        <v>2.4423</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3948,10 +3948,10 @@
         <v>2100</v>
       </c>
       <c r="F134" s="1">
-        <v>6.17</v>
+        <v>6.13</v>
       </c>
       <c r="G134" s="2">
-        <v>2.9381</v>
+        <v>2.919</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3971,10 +3971,10 @@
         <v>2200</v>
       </c>
       <c r="F135" s="1">
-        <v>5.68</v>
+        <v>5.51</v>
       </c>
       <c r="G135" s="2">
-        <v>2.5818</v>
+        <v>2.5045</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3994,10 +3994,10 @@
         <v>3100</v>
       </c>
       <c r="F136" s="1">
-        <v>4.86</v>
+        <v>5.05</v>
       </c>
       <c r="G136" s="2">
-        <v>1.5677</v>
+        <v>1.629</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4033,10 +4033,10 @@
         <v>4800</v>
       </c>
       <c r="F138" s="1">
-        <v>7.62</v>
+        <v>7.94</v>
       </c>
       <c r="G138" s="2">
-        <v>1.5875</v>
+        <v>1.6542</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4056,10 +4056,10 @@
         <v>5700</v>
       </c>
       <c r="F139" s="1">
-        <v>9.15</v>
+        <v>8.26</v>
       </c>
       <c r="G139" s="2">
-        <v>1.6053</v>
+        <v>1.4491</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4079,10 +4079,10 @@
         <v>5700</v>
       </c>
       <c r="F140" s="1">
-        <v>7.62</v>
+        <v>7.51</v>
       </c>
       <c r="G140" s="2">
-        <v>1.3368</v>
+        <v>1.3175</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4102,10 +4102,10 @@
         <v>4900</v>
       </c>
       <c r="F141" s="1">
-        <v>7.57</v>
+        <v>7.31</v>
       </c>
       <c r="G141" s="2">
-        <v>1.5449</v>
+        <v>1.4918</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -4125,10 +4125,10 @@
         <v>3100</v>
       </c>
       <c r="F142" s="1">
-        <v>7.25</v>
+        <v>6.87</v>
       </c>
       <c r="G142" s="2">
-        <v>2.3387</v>
+        <v>2.2161</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4148,10 +4148,10 @@
         <v>4700</v>
       </c>
       <c r="F143" s="1">
-        <v>7.09</v>
+        <v>6.47</v>
       </c>
       <c r="G143" s="2">
-        <v>1.5085</v>
+        <v>1.3766</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -4171,10 +4171,10 @@
         <v>3900</v>
       </c>
       <c r="F144" s="1">
-        <v>5.87</v>
+        <v>5.75</v>
       </c>
       <c r="G144" s="2">
-        <v>1.5051</v>
+        <v>1.4744</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -4194,10 +4194,10 @@
         <v>2600</v>
       </c>
       <c r="F145" s="1">
-        <v>5.12</v>
+        <v>5.37</v>
       </c>
       <c r="G145" s="2">
-        <v>1.9692</v>
+        <v>2.0654</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -4233,10 +4233,10 @@
         <v>3500</v>
       </c>
       <c r="F147" s="1">
-        <v>8.029999999999999</v>
+        <v>7.75</v>
       </c>
       <c r="G147" s="2">
-        <v>2.2943</v>
+        <v>2.2143</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -4256,401 +4256,378 @@
         <v>2500</v>
       </c>
       <c r="F148" s="1">
-        <v>8.699999999999999</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="G148" s="2">
-        <v>3.48</v>
+        <v>3.488</v>
       </c>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B149" t="s">
         <v>183</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D149" t="s">
         <v>9</v>
       </c>
       <c r="E149">
-        <v>2500</v>
+        <v>3600</v>
       </c>
       <c r="F149" s="1">
-        <v>10.27</v>
+        <v>8.31</v>
       </c>
       <c r="G149" s="2">
-        <v>4.108</v>
+        <v>2.3083</v>
       </c>
     </row>
     <row r="150" spans="1:7">
       <c r="A150" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B150" t="s">
         <v>183</v>
       </c>
       <c r="C150">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E150">
-        <v>3600</v>
+        <v>3500</v>
       </c>
       <c r="F150" s="1">
-        <v>8.630000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="G150" s="2">
-        <v>2.3972</v>
+        <v>2.3371</v>
       </c>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B151" t="s">
         <v>183</v>
       </c>
       <c r="C151">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E151">
-        <v>3500</v>
+        <v>2900</v>
       </c>
       <c r="F151" s="1">
-        <v>8.07</v>
+        <v>7.31</v>
       </c>
       <c r="G151" s="2">
-        <v>2.3057</v>
+        <v>2.5207</v>
       </c>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B152" t="s">
         <v>183</v>
       </c>
       <c r="C152">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D152" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E152">
-        <v>2900</v>
+        <v>3700</v>
       </c>
       <c r="F152" s="1">
-        <v>7.63</v>
+        <v>6.86</v>
       </c>
       <c r="G152" s="2">
-        <v>2.631</v>
+        <v>1.8541</v>
       </c>
     </row>
     <row r="153" spans="1:7">
       <c r="A153" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B153" t="s">
         <v>183</v>
       </c>
       <c r="C153">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D153" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E153">
-        <v>3700</v>
+        <v>3000</v>
       </c>
       <c r="F153" s="1">
-        <v>7.61</v>
+        <v>6.66</v>
       </c>
       <c r="G153" s="2">
-        <v>2.0568</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="154" spans="1:7">
       <c r="A154" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B154" t="s">
         <v>183</v>
       </c>
       <c r="C154">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D154" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E154">
-        <v>3000</v>
+        <v>2900</v>
       </c>
       <c r="F154" s="1">
-        <v>6.13</v>
+        <v>6.79</v>
       </c>
       <c r="G154" s="2">
-        <v>2.0433</v>
+        <v>2.3414</v>
       </c>
     </row>
     <row r="155" spans="1:7">
       <c r="A155" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B155" t="s">
         <v>183</v>
       </c>
       <c r="C155">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D155" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E155">
         <v>2900</v>
       </c>
       <c r="F155" s="1">
-        <v>5.91</v>
+        <v>6.57</v>
       </c>
       <c r="G155" s="2">
-        <v>2.0379</v>
+        <v>2.2655</v>
       </c>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B156" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="C156">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D156" t="s">
         <v>9</v>
       </c>
       <c r="E156">
-        <v>2900</v>
+        <v>5200</v>
       </c>
       <c r="F156" s="1">
-        <v>6.54</v>
+        <v>8.19</v>
       </c>
       <c r="G156" s="2">
-        <v>2.2552</v>
+        <v>1.575</v>
       </c>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B157" t="s">
         <v>193</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D157" t="s">
         <v>9</v>
       </c>
       <c r="E157">
-        <v>5200</v>
+        <v>4000</v>
       </c>
       <c r="F157" s="1">
-        <v>7.69</v>
+        <v>8.73</v>
       </c>
       <c r="G157" s="2">
-        <v>1.4788</v>
+        <v>2.1825</v>
       </c>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B158" t="s">
         <v>193</v>
       </c>
       <c r="C158">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D158" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E158">
-        <v>4000</v>
+        <v>5300</v>
       </c>
       <c r="F158" s="1">
-        <v>8.59</v>
+        <v>8.41</v>
       </c>
       <c r="G158" s="2">
-        <v>2.1475</v>
+        <v>1.5868</v>
       </c>
     </row>
     <row r="159" spans="1:7">
       <c r="A159" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B159" t="s">
         <v>193</v>
       </c>
       <c r="C159">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E159">
-        <v>5300</v>
+        <v>3600</v>
       </c>
       <c r="F159" s="1">
-        <v>9.01</v>
+        <v>7.41</v>
       </c>
       <c r="G159" s="2">
-        <v>1.7</v>
+        <v>2.0583</v>
       </c>
     </row>
     <row r="160" spans="1:7">
       <c r="A160" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B160" t="s">
         <v>193</v>
       </c>
       <c r="C160">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D160" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E160">
-        <v>3600</v>
+        <v>5200</v>
       </c>
       <c r="F160" s="1">
-        <v>8.460000000000001</v>
+        <v>7.17</v>
       </c>
       <c r="G160" s="2">
-        <v>2.35</v>
+        <v>1.3788</v>
       </c>
     </row>
     <row r="161" spans="1:7">
       <c r="A161" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B161" t="s">
         <v>193</v>
       </c>
       <c r="C161">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D161" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E161">
-        <v>5200</v>
+        <v>2800</v>
       </c>
       <c r="F161" s="1">
-        <v>7.33</v>
+        <v>7.44</v>
       </c>
       <c r="G161" s="2">
-        <v>1.4096</v>
+        <v>2.6571</v>
       </c>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B162" t="s">
         <v>193</v>
       </c>
       <c r="C162">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D162" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E162">
-        <v>2800</v>
+        <v>4100</v>
       </c>
       <c r="F162" s="1">
-        <v>7.68</v>
+        <v>6.61</v>
       </c>
       <c r="G162" s="2">
-        <v>2.7429</v>
+        <v>1.6122</v>
       </c>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B163" t="s">
         <v>193</v>
       </c>
       <c r="C163">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D163" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E163">
-        <v>4100</v>
+        <v>2100</v>
       </c>
       <c r="F163" s="1">
-        <v>6.56</v>
+        <v>5.47</v>
       </c>
       <c r="G163" s="2">
-        <v>1.6</v>
+        <v>2.6048</v>
       </c>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B164" t="s">
         <v>193</v>
       </c>
       <c r="C164">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D164" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E164">
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="F164" s="1">
-        <v>5.32</v>
+        <v>1.54</v>
       </c>
       <c r="G164" s="2">
-        <v>2.5333</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7">
-      <c r="A165" t="s">
-        <v>201</v>
-      </c>
-      <c r="B165" t="s">
-        <v>193</v>
-      </c>
-      <c r="C165">
-        <v>9</v>
-      </c>
-      <c r="D165" t="s">
-        <v>9</v>
-      </c>
-      <c r="E165">
-        <v>2400</v>
-      </c>
-      <c r="F165" s="1">
-        <v>5.86</v>
-      </c>
-      <c r="G165" s="2">
-        <v>2.4417</v>
+        <v>0.6417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>